<commit_message>
hide a few columns
</commit_message>
<xml_diff>
--- a/sample-data/Payroll_Options.xlsx
+++ b/sample-data/Payroll_Options.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Code\GitHub\dashboard2\sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C782DC-07ED-482B-8494-8FC52BF24AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29797E98-A4E5-4FB0-84C5-2AE731577E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="2745" windowWidth="25785" windowHeight="11295" xr2:uid="{BF50A21A-9D10-4D59-A197-EBA26977D54B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF50A21A-9D10-4D59-A197-EBA26977D54B}"/>
   </bookViews>
   <sheets>
     <sheet name="Rates" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Holiday</t>
   </si>
   <si>
-    <t>Provider Test</t>
-  </si>
-  <si>
     <t>Patient Name</t>
   </si>
   <si>
@@ -87,10 +84,22 @@
     <t>Limit</t>
   </si>
   <si>
-    <t>Patient Test</t>
-  </si>
-  <si>
-    <t>Test, Lora</t>
+    <t>Test Value</t>
+  </si>
+  <si>
+    <t>Test Value2</t>
+  </si>
+  <si>
+    <t>John Test</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Bob Doe</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
   </si>
 </sst>
 </file>
@@ -462,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677DD7D-DFFA-4B2B-ACCB-71019CBA7542}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -524,7 +533,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -537,6 +546,57 @@
       </c>
       <c r="E4">
         <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -578,9 +638,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3DD269-ED99-4FDA-AA03-92E668C828C3}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -590,24 +652,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -633,15 +684,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>